<commit_message>
xlsx : updata & func : 0x00 find end of text & gui : disable btn at init
</commit_message>
<xml_diff>
--- a/오프셋별화자이름.xlsx
+++ b/오프셋별화자이름.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sg000\Desktop\play\KRTrans\DGMAdv KR\21sincedStartFirst\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sg000\Desktop\play\KRTrans\DGMAdv KR\21sincedStartFirst\locale_kr\gui\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F46AB2-9BAB-4E42-BAFF-16FF470D3642}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3433F8A-882A-4A54-A1A9-FD370E7DB77C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="2868" windowWidth="23256" windowHeight="13176" xr2:uid="{687A896C-F325-48FE-96D3-7C93BFBE9C2B}"/>
+    <workbookView xWindow="12720" yWindow="1440" windowWidth="15165" windowHeight="13245" xr2:uid="{687A896C-F325-48FE-96D3-7C93BFBE9C2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$C$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$C$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>아나운서</t>
   </si>
@@ -141,6 +141,150 @@
   </si>
   <si>
     <t>누메몬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>핏코로몬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가지몬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>에테몬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>티라노몬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>겐나이</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>코카토리몬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>피요몬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>토게몬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>푸카몬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그레이몬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메탈그레이몬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>워그레이몬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가부몬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가루루몬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>워가루루몬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메탈가루루몬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>버드라몬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가루다몬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>호우오우몬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>캅테리몬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아트라캅테리몬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>헤라클캅테리몬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리리몬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로제몬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>고마몬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>잇카쿠몬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>즈도몬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>바이크몬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>엔제몬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>홀리엔제몬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>세라피몬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>플롯트몬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>테일몬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>엔제우몬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오파니몬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>반데몬</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -514,10 +658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0244602D-8921-4897-ACAB-30DBFD651690}">
-  <dimension ref="B1:C31"/>
+  <dimension ref="B1:C66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -609,162 +753,442 @@
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B12" s="2">
-        <v>2211</v>
+        <v>2131</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B13" s="2">
-        <v>2311</v>
+        <v>2141</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B14" s="2">
-        <v>2411</v>
+        <v>2151</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B15" s="2">
-        <v>2421</v>
+        <v>2211</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B16" s="2">
-        <v>2511</v>
+        <v>2221</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" s="2">
-        <v>2521</v>
+        <v>2231</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" s="2">
-        <v>2611</v>
+        <v>2241</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" s="2">
-        <v>2711</v>
+        <v>2251</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" s="2">
-        <v>2721</v>
+        <v>2311</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" s="2">
-        <v>2811</v>
+        <v>2321</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" s="2">
-        <v>4902</v>
+        <v>2331</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B23" s="2">
-        <v>4903</v>
+        <v>2341</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B24" s="2">
-        <v>6061</v>
+        <v>2351</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B25" s="2">
-        <v>9003</v>
+        <v>2411</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B26" s="2">
-        <v>65535</v>
+        <v>2421</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B27" s="2">
-        <v>9001</v>
+        <v>2431</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B28" s="2">
-        <v>4071</v>
+        <v>2441</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B29" s="2">
-        <v>4061</v>
+        <v>2451</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B30" s="2">
-        <v>3011</v>
+        <v>2511</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B31" s="2">
+        <v>2521</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B32" s="2">
+        <v>2531</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B33" s="2">
+        <v>2541</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B34" s="2">
+        <v>2551</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B35" s="2">
+        <v>2611</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B36" s="2">
+        <v>2621</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B37" s="2">
+        <v>2631</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B38" s="2">
+        <v>2641</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B39" s="2">
+        <v>2651</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B40" s="2">
+        <v>2711</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B41" s="2">
+        <v>2721</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B42" s="2">
+        <v>2731</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B43" s="2">
+        <v>2741</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B44" s="2">
+        <v>2751</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B45" s="2">
+        <v>2811</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B46" s="2">
+        <v>2821</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B47" s="2">
+        <v>2831</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B48" s="2">
+        <v>2841</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B49" s="2">
+        <v>2851</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B50" s="2">
+        <v>3011</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B51" s="2">
+        <v>3021</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B52" s="2">
+        <v>3031</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B53" s="2">
         <v>4031</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C53" s="1" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B54" s="2">
+        <v>4061</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B55" s="2">
+        <v>4071</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B56" s="2">
+        <v>4182</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B57" s="2">
+        <v>4191</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B58" s="2">
+        <v>4201</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B59" s="2">
+        <v>4902</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B60" s="2">
+        <v>4903</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B61" s="2">
+        <v>4905</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B62" s="2">
+        <v>5011</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B63" s="2">
+        <v>6061</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B64" s="2">
+        <v>9001</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B65" s="2">
+        <v>9003</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B66" s="2">
+        <v>65535</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>